<commit_message>
HAJ-1 updating health validators and adding applicant ritual validators
</commit_message>
<xml_diff>
--- a/shj-admin-portal-web/src/main/resources/templates/excel/6/applicant-ritual-data.xlsx
+++ b/shj-admin-portal-web/src/main/resources/templates/excel/6/applicant-ritual-data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tasks\Hajj Initiative\excel template\excel\6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dev\projects\hajj\code\smart-hajj-admin-portal\shj-admin-portal-web\src\main\resources\templates\excel\6\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>ID Number 
 	رقم الهوية الوطنية / الإقامة</t>
@@ -40,10 +40,6 @@
   <si>
     <t>InsuranceNumber
 رقم بولصة التأمين</t>
-  </si>
-  <si>
-    <t>PermiNnumber
-	رقم التصريح</t>
   </si>
   <si>
     <t>VisaNumber
@@ -90,11 +86,6 @@
 DD/MM/YYYY</t>
   </si>
   <si>
-    <t>HijriSeason
-موسم الشعيرة
-YYYY</t>
-  </si>
-  <si>
     <t>DateOfBirthHijri
 	تاريخ الميلاد هجري
 YYYYMMDD</t>
@@ -107,6 +98,18 @@
   <si>
     <t>TafweegNumber
 رقم الفوج</t>
+  </si>
+  <si>
+    <t>BusNumber
+رقم الحافلة</t>
+  </si>
+  <si>
+    <t>SeatNumber
+رقم المقعد</t>
+  </si>
+  <si>
+    <t>PermitNumber
+	رقم التصريح</t>
   </si>
 </sst>
 </file>
@@ -266,295 +269,321 @@
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </left>
+        <right style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </right>
+        <top style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1" tint="0.14999847407452621"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="1" tint="0.14999847407452621"/>
         </left>
         <right/>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
-        <top style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </left>
-        <right style="thin">
-          <color theme="1" tint="0.14999847407452621"/>
-        </right>
         <top style="thin">
           <color theme="1" tint="0.14999847407452621"/>
         </top>
@@ -742,28 +771,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="B3:T31" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19" headerRowCellStyle="20% - Accent1">
-  <autoFilter ref="B3:T31"/>
-  <tableColumns count="19">
-    <tableColumn id="2" name="ID Number _x000a__x0009_رقم الهوية الوطنية / الإقامة" dataDxfId="18"/>
-    <tableColumn id="3" name="PassportNo_x000a__x0009_رقم الجواز" dataDxfId="17"/>
-    <tableColumn id="4" name="DateOfBirth_x000a__x0009_تاريخ الميلاد_x000a_DD/MM/YYYY" dataDxfId="16"/>
-    <tableColumn id="5" name="DateOfBirthHijri_x000a__x0009_تاريخ الميلاد هجري_x000a_YYYYMMDD" dataDxfId="15"/>
-    <tableColumn id="7" name="HamlahPackageCode_x000a_باقة الشركة" dataDxfId="14"/>
-    <tableColumn id="20" name="TafweegNumber_x000a_رقم الفوج" dataDxfId="0"/>
-    <tableColumn id="6" name="HijriSeason_x000a_موسم الشعيرة_x000a_YYYY" dataDxfId="13"/>
-    <tableColumn id="1" name="DateStartGregorian_x000a_تاريخ بداية الشعيرة ميلادي_x000a_DD/MM/YYYY" dataDxfId="12"/>
-    <tableColumn id="8" name="DateEndGregorian_x000a_تاريخ نهاية الشعيرة ميلادي_x000a_DD/MM/YYYY" dataDxfId="11"/>
-    <tableColumn id="9" name="DateStartHijri_x000a_تاريخ بداية الشعيرة هجري_x000a_YYYYMMDD" dataDxfId="10"/>
-    <tableColumn id="10" name="DateEndHijri_x000a_تاريخ نهاية الشعيرة هجري_x000a_YYYYMMDD" dataDxfId="9"/>
-    <tableColumn id="11" name="TypeCode_x000a__x0009_نوع الشعيرة" dataDxfId="8"/>
-    <tableColumn id="12" name="VisaNumber_x000a__x0009_رقم التأشيرة" dataDxfId="7"/>
-    <tableColumn id="13" name="PermiNnumber_x000a__x0009_رقم التصريح" dataDxfId="6"/>
-    <tableColumn id="14" name="InsuranceNumber_x000a_رقم بولصة التأمين" dataDxfId="5"/>
-    <tableColumn id="15" name="BorderNumber_x000a_رقم الحدود" dataDxfId="4"/>
-    <tableColumn id="16" name="Zone_x000a_النطاق" dataDxfId="3"/>
-    <tableColumn id="17" name="Group_x000a_المجموعة" dataDxfId="2"/>
-    <tableColumn id="18" name="Unit_x000a_الوحدة" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="B3:U31" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20" headerRowCellStyle="20% - Accent1">
+  <autoFilter ref="B3:U31"/>
+  <tableColumns count="20">
+    <tableColumn id="2" name="ID Number _x000a__x0009_رقم الهوية الوطنية / الإقامة" dataDxfId="19"/>
+    <tableColumn id="3" name="PassportNo_x000a__x0009_رقم الجواز" dataDxfId="18"/>
+    <tableColumn id="4" name="DateOfBirth_x000a__x0009_تاريخ الميلاد_x000a_DD/MM/YYYY" dataDxfId="17"/>
+    <tableColumn id="5" name="DateOfBirthHijri_x000a__x0009_تاريخ الميلاد هجري_x000a_YYYYMMDD" dataDxfId="16"/>
+    <tableColumn id="7" name="HamlahPackageCode_x000a_باقة الشركة" dataDxfId="15"/>
+    <tableColumn id="20" name="TafweegNumber_x000a_رقم الفوج" dataDxfId="14"/>
+    <tableColumn id="1" name="DateStartGregorian_x000a_تاريخ بداية الشعيرة ميلادي_x000a_DD/MM/YYYY" dataDxfId="13"/>
+    <tableColumn id="8" name="DateEndGregorian_x000a_تاريخ نهاية الشعيرة ميلادي_x000a_DD/MM/YYYY" dataDxfId="12"/>
+    <tableColumn id="9" name="DateStartHijri_x000a_تاريخ بداية الشعيرة هجري_x000a_YYYYMMDD" dataDxfId="11"/>
+    <tableColumn id="10" name="DateEndHijri_x000a_تاريخ نهاية الشعيرة هجري_x000a_YYYYMMDD" dataDxfId="10"/>
+    <tableColumn id="11" name="TypeCode_x000a__x0009_نوع الشعيرة" dataDxfId="9"/>
+    <tableColumn id="12" name="VisaNumber_x000a__x0009_رقم التأشيرة" dataDxfId="8"/>
+    <tableColumn id="13" name="PermitNumber_x000a__x0009_رقم التصريح" dataDxfId="7"/>
+    <tableColumn id="14" name="InsuranceNumber_x000a_رقم بولصة التأمين" dataDxfId="6"/>
+    <tableColumn id="15" name="BorderNumber_x000a_رقم الحدود" dataDxfId="5"/>
+    <tableColumn id="16" name="Zone_x000a_النطاق" dataDxfId="4"/>
+    <tableColumn id="17" name="Group_x000a_المجموعة" dataDxfId="3"/>
+    <tableColumn id="18" name="Unit_x000a_الوحدة" dataDxfId="2"/>
+    <tableColumn id="19" name="BusNumber_x000a_رقم الحافلة" dataDxfId="1"/>
+    <tableColumn id="21" name="SeatNumber_x000a_رقم المقعد" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1032,31 +1062,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:T31"/>
+  <dimension ref="B3:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="5" width="21.26953125" customWidth="1"/>
-    <col min="6" max="7" width="22.54296875" customWidth="1"/>
-    <col min="8" max="8" width="21.26953125" customWidth="1"/>
-    <col min="9" max="9" width="22.54296875" customWidth="1"/>
-    <col min="10" max="10" width="21.26953125" customWidth="1"/>
-    <col min="11" max="11" width="22.54296875" customWidth="1"/>
-    <col min="12" max="12" width="21.26953125" customWidth="1"/>
-    <col min="13" max="13" width="22.54296875" customWidth="1"/>
-    <col min="14" max="14" width="21.26953125" customWidth="1"/>
-    <col min="15" max="15" width="22.54296875" customWidth="1"/>
-    <col min="16" max="17" width="21.26953125" customWidth="1"/>
-    <col min="18" max="18" width="13.81640625" customWidth="1"/>
-    <col min="19" max="19" width="13.36328125" customWidth="1"/>
-    <col min="20" max="20" width="12.90625" customWidth="1"/>
+    <col min="2" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="8" width="22.5703125" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" customWidth="1"/>
+    <col min="12" max="19" width="21.42578125" customWidth="1"/>
+    <col min="20" max="21" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:20" s="2" customFormat="1" ht="46.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:21" s="2" customFormat="1" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1064,46 +1087,46 @@
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="H3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>2</v>
       </c>
       <c r="R3" s="7" t="s">
         <v>8</v>
@@ -1112,17 +1135,20 @@
         <v>9</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="3"/>
+      <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
@@ -1131,19 +1157,20 @@
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
       <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
+      <c r="Q4" s="13"/>
       <c r="R4" s="13"/>
       <c r="S4" s="13"/>
       <c r="T4" s="13"/>
-    </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U4" s="13"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="3"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
@@ -1152,19 +1179,20 @@
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
+      <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U5" s="3"/>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
-      <c r="H6" s="3"/>
+      <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -1173,19 +1201,20 @@
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
+      <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U6" s="3"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="3"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
@@ -1194,19 +1223,20 @@
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
+      <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U7" s="3"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="3"/>
+      <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -1215,19 +1245,20 @@
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
+      <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
-    </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U8" s="3"/>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="3"/>
+      <c r="H9" s="9"/>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
@@ -1236,19 +1267,20 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
+      <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U9" s="3"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="3"/>
+      <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
@@ -1257,19 +1289,20 @@
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
+      <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U10" s="3"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="3"/>
+      <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
@@ -1278,19 +1311,20 @@
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
+      <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U11" s="3"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="3"/>
+      <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -1299,19 +1333,20 @@
       <c r="N12" s="8"/>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
+      <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U12" s="3"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="3"/>
+      <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
@@ -1320,19 +1355,20 @@
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
+      <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
-    </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U13" s="3"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="3"/>
+      <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -1341,19 +1377,20 @@
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
+      <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U14" s="3"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="3"/>
+      <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
@@ -1362,19 +1399,20 @@
       <c r="N15" s="9"/>
       <c r="O15" s="9"/>
       <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
+      <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U15" s="3"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="3"/>
+      <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
@@ -1383,19 +1421,20 @@
       <c r="N16" s="8"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
+      <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
-    </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U16" s="3"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="3"/>
+      <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
@@ -1404,19 +1443,20 @@
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
       <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
+      <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
-    </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U17" s="3"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="3"/>
+      <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -1425,19 +1465,20 @@
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
+      <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
-    </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U18" s="3"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="3"/>
+      <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
@@ -1446,19 +1487,20 @@
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
       <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
+      <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
-    </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U19" s="3"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="3"/>
+      <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -1467,19 +1509,20 @@
       <c r="N20" s="8"/>
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
+      <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
-    </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U20" s="3"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="3"/>
+      <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -1488,19 +1531,20 @@
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
+      <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
-    </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U21" s="3"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="3"/>
+      <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -1509,19 +1553,20 @@
       <c r="N22" s="8"/>
       <c r="O22" s="8"/>
       <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
+      <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
-    </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U22" s="3"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="3"/>
+      <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -1530,19 +1575,20 @@
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
+      <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
-    </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U23" s="3"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
-      <c r="H24" s="3"/>
+      <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
@@ -1551,19 +1597,20 @@
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
       <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
+      <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
-    </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U24" s="3"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="3"/>
+      <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
@@ -1572,19 +1619,20 @@
       <c r="N25" s="9"/>
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
+      <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
-    </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U25" s="3"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="3"/>
+      <c r="H26" s="8"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
@@ -1593,19 +1641,20 @@
       <c r="N26" s="8"/>
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
+      <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
-    </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U26" s="3"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="3"/>
+      <c r="H27" s="9"/>
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
@@ -1614,19 +1663,20 @@
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
       <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
+      <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
-    </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U27" s="3"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="3"/>
+      <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
@@ -1635,19 +1685,20 @@
       <c r="N28" s="8"/>
       <c r="O28" s="8"/>
       <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
+      <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
-    </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U28" s="3"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="H29" s="3"/>
+      <c r="H29" s="9"/>
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
@@ -1656,19 +1707,20 @@
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
+      <c r="Q29" s="3"/>
       <c r="R29" s="3"/>
       <c r="S29" s="3"/>
       <c r="T29" s="3"/>
-    </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U29" s="3"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
-      <c r="H30" s="3"/>
+      <c r="H30" s="8"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
@@ -1677,19 +1729,20 @@
       <c r="N30" s="8"/>
       <c r="O30" s="8"/>
       <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
+      <c r="Q30" s="3"/>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
-    </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="U30" s="3"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="5"/>
+      <c r="H31" s="11"/>
       <c r="I31" s="11"/>
       <c r="J31" s="11"/>
       <c r="K31" s="11"/>
@@ -1698,10 +1751,11 @@
       <c r="N31" s="11"/>
       <c r="O31" s="11"/>
       <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
+      <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
       <c r="S31" s="5"/>
       <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1767,7 +1821,7 @@
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFE8DB3C-0EC7-4FB7-AAED-3D6AD2FBFBBE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4D937D1-0DDB-4077-9CC8-78E737629F7D}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
template files:Sheet name same for applicant health data and applicant ritual data excel workbooks and fixed some issues related to UI in printing request HAJ-212 ,HAJJ-206
</commit_message>
<xml_diff>
--- a/shj-admin-portal-web/src/main/resources/templates/excel/6/applicant-ritual-data.xlsx
+++ b/shj-admin-portal-web/src/main/resources/templates/excel/6/applicant-ritual-data.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dev\projects\hajj\code\smart-hajj-admin-portal\shj-admin-portal-web\src\main\resources\templates\excel\6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ELM\Smart Hajj\Smart Hajj Admin\git\smart-hajj\shj-admin-portal-web\src\main\resources\templates\excel\6\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
-    <sheet name="Applicant Health Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Applicant Ritual Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1767,11 +1767,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%HOSTNAME%">N14946.elm.com.sa</XMLData>
+<XMLData TextToDisplay="%USERNAME%">adhaoui</XMLData>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">09:57 11/05/2021</XMLData>
+<XMLData TextToDisplay="%EMAILADDRESS%">adhaoui@elm.sa</XMLData>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1779,11 +1779,11 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%EMAILADDRESS%">adhaoui@elm.sa</XMLData>
+<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">09:57 11/05/2021</XMLData>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%USERNAME%">adhaoui</XMLData>
+<XMLData TextToDisplay="%HOSTNAME%">N14946.elm.com.sa</XMLData>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1791,13 +1791,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F4A07F7-3973-4838-B7E7-EB7D8745504A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E27E3D3-165F-47EA-86B0-A6D84A589584}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03A4FEA3-53F1-4DDC-9022-BAA5D30164C7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{751C11B0-08C1-4EE8-9007-1CCB88EBD376}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
@@ -1809,13 +1809,13 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{751C11B0-08C1-4EE8-9007-1CCB88EBD376}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03A4FEA3-53F1-4DDC-9022-BAA5D30164C7}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E27E3D3-165F-47EA-86B0-A6D84A589584}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F4A07F7-3973-4838-B7E7-EB7D8745504A}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>

</xml_diff>